<commit_message>
Update spanish translation files and databooks
</commit_message>
<xml_diff>
--- a/inputs/es/LiST countries/AFG_databook.xlsx
+++ b/inputs/es/LiST countries/AFG_databook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\0B2k5hvlxN8FnTm9fb1c2alB2cjQ\Optima\Optima Nutrition\Development\LiST Optima bridge\App\es\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BDD9CC7-BFB6-4B9D-B2FD-F384B94074D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC637574-3000-4E2B-8962-9C23A23BF1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="10" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entradas de población-año base" sheetId="1" r:id="rId1"/>
@@ -963,7 +963,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="344">
   <si>
     <t>Datos del año de referencia</t>
   </si>
@@ -1577,10 +1577,10 @@
     <t>Condición</t>
   </si>
   <si>
-    <t>Malnutrición aguda moderada (MAM)</t>
+    <t>MAM</t>
   </si>
   <si>
-    <t>Malnutrición Aguda Severa (MAS)</t>
+    <t>SAM</t>
   </si>
   <si>
     <t>Amplio grupo de población</t>
@@ -1787,6 +1787,9 @@
     <t>Estado de la peso para la talla (WHZ)</t>
   </si>
   <si>
+    <t>MAS</t>
+  </si>
+  <si>
     <t>Riesgo relativo de las causas de muerte según el estado de la anemia</t>
   </si>
   <si>
@@ -1986,6 +1989,12 @@
   </si>
   <si>
     <t>Efectividad en incidencia</t>
+  </si>
+  <si>
+    <t>Malnutrición Aguda Severa (MAS)</t>
+  </si>
+  <si>
+    <t>Malnutrición aguda moderada (MAM)</t>
   </si>
 </sst>
 </file>
@@ -2487,12 +2496,12 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -3133,7 +3142,7 @@
       <c r="B30" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="103">
+      <c r="C30" s="102">
         <v>9.447220278431899E-2</v>
       </c>
     </row>
@@ -3141,7 +3150,7 @@
       <c r="B31" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="103">
+      <c r="C31" s="102">
         <v>0.167430435799206</v>
       </c>
     </row>
@@ -3149,7 +3158,7 @@
       <c r="B32" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="103">
+      <c r="C32" s="102">
         <v>0.54575654665008</v>
       </c>
     </row>
@@ -4564,7 +4573,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4665,7 +4674,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oCcRVZRVedfmPDxbHCUa1ha0G24FDzw2IMjTX9h9tZFpzudyFVu9UT7WzHBNxO0XVPbOKfliHBIYMSvq4TYM/g==" saltValue="Hsf1tSKIw5dAi8qT4gu3LQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="UwLpYKH4JCcE8Xq2IHJhvub/xD9AgH0IM4lV/9WRHgCSUxzpV8fBT3xa99cPLYJiF0GQRGEFzK/9+ANqj+gVIQ==" saltValue="Rz7LhHchEqdsBP8cBVtfDA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -11064,7 +11073,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C17" s="67" t="s">
@@ -11422,7 +11431,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="102" t="s">
+      <c r="B34" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C34" s="67" t="s">
@@ -11780,7 +11789,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C51" s="67" t="s">
@@ -12244,7 +12253,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="102" t="s">
+      <c r="B70" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C70" s="67" t="s">
@@ -12682,7 +12691,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="102" t="s">
+      <c r="B87" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C87" s="67" t="s">
@@ -13120,7 +13129,7 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="102" t="s">
+      <c r="B104" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C104" s="67" t="s">
@@ -13589,7 +13598,7 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="102" t="s">
+      <c r="B123" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C123" s="67" t="s">
@@ -14027,7 +14036,7 @@
       </c>
     </row>
     <row r="140" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="102" t="s">
+      <c r="B140" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C140" s="67" t="s">
@@ -14465,7 +14474,7 @@
       </c>
     </row>
     <row r="157" spans="2:8" ht="13" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="102" t="s">
+      <c r="B157" s="103" t="s">
         <v>149</v>
       </c>
       <c r="C157" s="67" t="s">
@@ -15773,8 +15782,8 @@
   </sheetPr>
   <dimension ref="A1:P328"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16648,7 +16657,7 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C33" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D33" s="90">
         <v>1</v>
@@ -16763,7 +16772,7 @@
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C37" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D37" s="90">
         <v>1</v>
@@ -16878,7 +16887,7 @@
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C41" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D41" s="90">
         <v>1</v>
@@ -16993,7 +17002,7 @@
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C45" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D45" s="90">
         <v>1</v>
@@ -17108,7 +17117,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C49" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D49" s="90">
         <v>1</v>
@@ -17223,7 +17232,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C53" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D53" s="90">
         <v>1</v>
@@ -17255,7 +17264,7 @@
     </row>
     <row r="55" spans="1:16" s="70" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="60" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -17266,7 +17275,7 @@
         <v>265</v>
       </c>
       <c r="C56" s="80" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D56" s="62" t="s">
         <v>112</v>
@@ -17292,7 +17301,7 @@
         <v>91</v>
       </c>
       <c r="C57" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D57" s="89">
         <v>1</v>
@@ -17314,7 +17323,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D58" s="90">
         <v>10.675000000000001</v>
@@ -17339,7 +17348,7 @@
         <v>92</v>
       </c>
       <c r="C59" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D59" s="89">
         <v>1</v>
@@ -17361,7 +17370,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D60" s="90">
         <v>10.675000000000001</v>
@@ -17386,7 +17395,7 @@
         <v>93</v>
       </c>
       <c r="C61" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D61" s="89">
         <v>1</v>
@@ -17408,7 +17417,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D62" s="90">
         <v>10.675000000000001</v>
@@ -17434,7 +17443,7 @@
     </row>
     <row r="64" spans="1:16" s="70" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="60" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -17445,7 +17454,7 @@
         <v>265</v>
       </c>
       <c r="C65" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D65" s="62" t="s">
         <v>67</v>
@@ -18509,7 +18518,7 @@
     </row>
     <row r="103" spans="1:16" s="70" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.3">
@@ -18520,7 +18529,7 @@
         <v>122</v>
       </c>
       <c r="C104" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D104" s="62" t="s">
         <v>67</v>
@@ -19441,7 +19450,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C143" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D143" s="119">
         <f t="shared" si="3"/>
@@ -19544,7 +19553,7 @@
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C147" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D147" s="119">
         <f t="shared" si="3"/>
@@ -19647,7 +19656,7 @@
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C151" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D151" s="119">
         <f t="shared" si="4"/>
@@ -19750,7 +19759,7 @@
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C155" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D155" s="119">
         <f t="shared" si="4"/>
@@ -19853,7 +19862,7 @@
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C159" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D159" s="119">
         <f t="shared" si="4"/>
@@ -19956,7 +19965,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C163" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D163" s="119">
         <f t="shared" si="5"/>
@@ -19985,7 +19994,7 @@
     </row>
     <row r="165" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="60" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B165" s="70"/>
       <c r="C165" s="70"/>
@@ -20003,7 +20012,7 @@
         <v>265</v>
       </c>
       <c r="C166" s="80" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D166" s="62" t="s">
         <v>112</v>
@@ -20025,7 +20034,7 @@
         <v>91</v>
       </c>
       <c r="C167" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D167" s="119">
         <f t="shared" ref="D167:G172" si="6">D57*0.7</f>
@@ -20047,7 +20056,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C168" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D168" s="119">
         <f t="shared" si="6"/>
@@ -20072,7 +20081,7 @@
         <v>92</v>
       </c>
       <c r="C169" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D169" s="119">
         <f t="shared" si="6"/>
@@ -20094,7 +20103,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C170" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D170" s="119">
         <f t="shared" si="6"/>
@@ -20119,7 +20128,7 @@
         <v>93</v>
       </c>
       <c r="C171" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D171" s="119">
         <f t="shared" si="6"/>
@@ -20141,7 +20150,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C172" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D172" s="119">
         <f t="shared" si="6"/>
@@ -20167,7 +20176,7 @@
     </row>
     <row r="174" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="60" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B174" s="70"/>
       <c r="C174" s="70"/>
@@ -20185,7 +20194,7 @@
         <v>265</v>
       </c>
       <c r="C175" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D175" s="62" t="s">
         <v>67</v>
@@ -21097,7 +21106,7 @@
     </row>
     <row r="213" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B213" s="70"/>
       <c r="C213" s="70"/>
@@ -21115,7 +21124,7 @@
         <v>122</v>
       </c>
       <c r="C214" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D214" s="62" t="s">
         <v>67</v>
@@ -22043,7 +22052,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C253" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D253" s="119">
         <f t="shared" si="13"/>
@@ -22150,7 +22159,7 @@
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C257" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D257" s="119">
         <f t="shared" si="13"/>
@@ -22257,7 +22266,7 @@
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C261" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D261" s="119">
         <f t="shared" si="14"/>
@@ -22364,7 +22373,7 @@
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C265" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D265" s="119">
         <f t="shared" si="14"/>
@@ -22471,7 +22480,7 @@
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C269" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D269" s="119">
         <f t="shared" si="14"/>
@@ -22578,7 +22587,7 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C273" s="83" t="s">
-        <v>205</v>
+        <v>274</v>
       </c>
       <c r="D273" s="119">
         <f t="shared" si="15"/>
@@ -22608,7 +22617,7 @@
     </row>
     <row r="275" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="60" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B275" s="70"/>
       <c r="C275" s="70"/>
@@ -22627,7 +22636,7 @@
         <v>265</v>
       </c>
       <c r="C276" s="80" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D276" s="62" t="s">
         <v>112</v>
@@ -22649,7 +22658,7 @@
         <v>91</v>
       </c>
       <c r="C277" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D277" s="119">
         <f t="shared" ref="D277:G282" si="16">D57*1.2</f>
@@ -22671,7 +22680,7 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C278" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D278" s="119">
         <f t="shared" si="16"/>
@@ -22696,7 +22705,7 @@
         <v>92</v>
       </c>
       <c r="C279" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D279" s="119">
         <f t="shared" si="16"/>
@@ -22718,7 +22727,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C280" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D280" s="119">
         <f t="shared" si="16"/>
@@ -22743,7 +22752,7 @@
         <v>93</v>
       </c>
       <c r="C281" s="83" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D281" s="119">
         <f t="shared" si="16"/>
@@ -22765,7 +22774,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C282" s="83" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D282" s="119">
         <f t="shared" si="16"/>
@@ -22791,7 +22800,7 @@
     </row>
     <row r="284" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="60" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B284" s="70"/>
       <c r="C284" s="70"/>
@@ -22810,7 +22819,7 @@
         <v>265</v>
       </c>
       <c r="C285" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D285" s="62" t="s">
         <v>67</v>
@@ -23759,7 +23768,7 @@
     </row>
     <row r="323" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="60" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B323" s="70"/>
       <c r="C323" s="70"/>
@@ -23778,7 +23787,7 @@
         <v>122</v>
       </c>
       <c r="C324" s="80" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D324" s="62" t="s">
         <v>67</v>
@@ -23899,7 +23908,6 @@
       <c r="I328" s="78"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gHW1yfUCyQ+RwqESgWyh8TCcB78xhsFamj+CNDjioW160ilGJKQx2Rt4OfClUPypHH52sTIrprul6Zjcfdu5Ag==" saltValue="Imjwrw1LZZsi/oHsWCF3QA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -23912,7 +23920,7 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
@@ -23931,7 +23939,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="70" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -23957,10 +23965,10 @@
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="71" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" s="90" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D3" s="90">
         <v>45</v>
@@ -23978,7 +23986,7 @@
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57"/>
       <c r="B4" s="75" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C4" s="90">
         <v>1.0249999999999999</v>
@@ -23998,7 +24006,7 @@
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="63" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -24091,7 +24099,7 @@
     </row>
     <row r="11" spans="1:7" s="70" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="60" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -24121,7 +24129,7 @@
     </row>
     <row r="14" spans="1:7" s="70" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="60" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -24129,7 +24137,7 @@
         <v>272</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C15" s="90">
         <v>1.0249999999999999</v>
@@ -24150,7 +24158,7 @@
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="57"/>
       <c r="B16" s="75" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C16" s="90">
         <v>1.0249999999999999</v>
@@ -24173,7 +24181,7 @@
         <v>111</v>
       </c>
       <c r="B17" s="71" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C17" s="90">
         <v>1</v>
@@ -24194,7 +24202,7 @@
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" s="70" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="60" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="63" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -24235,7 +24243,7 @@
     </row>
     <row r="24" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B24" s="70"/>
       <c r="C24" s="70"/>
@@ -24267,10 +24275,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="71" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C26" s="90" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D26" s="90">
         <f t="shared" ref="D26:G27" si="0">D3*0.9</f>
@@ -24292,7 +24300,7 @@
     <row r="27" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="57"/>
       <c r="B27" s="75" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C27" s="90">
         <f>C4*0.9</f>
@@ -24317,12 +24325,12 @@
     </row>
     <row r="28" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="63" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="75" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C29" s="90">
         <f t="shared" ref="C29:G32" si="1">C6*0.9</f>
@@ -24347,7 +24355,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="75" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C30" s="90">
         <f t="shared" si="1"/>
@@ -24372,7 +24380,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="75" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C31" s="90">
         <f t="shared" si="1"/>
@@ -24397,7 +24405,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="75" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C32" s="90">
         <f t="shared" si="1"/>
@@ -24430,7 +24438,7 @@
     </row>
     <row r="34" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="60" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B34" s="70"/>
       <c r="C34" s="70"/>
@@ -24442,7 +24450,7 @@
     <row r="35" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="63"/>
       <c r="B35" s="71" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C35" s="90">
         <f>C12*0.9</f>
@@ -24468,7 +24476,7 @@
     </row>
     <row r="37" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="60" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B37" s="70"/>
       <c r="C37" s="70"/>
@@ -24482,7 +24490,7 @@
         <v>272</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C38" s="90">
         <f t="shared" ref="C38:G40" si="2">C15*0.9</f>
@@ -24508,7 +24516,7 @@
     <row r="39" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="57"/>
       <c r="B39" s="75" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C39" s="90">
         <f t="shared" si="2"/>
@@ -24536,7 +24544,7 @@
         <v>111</v>
       </c>
       <c r="B40" s="71" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C40" s="90">
         <f t="shared" si="2"/>
@@ -24561,7 +24569,7 @@
     </row>
     <row r="42" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="60" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B42" s="70"/>
       <c r="C42" s="70"/>
@@ -24589,7 +24597,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="71" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C44" s="90">
         <f>C21*0.9</f>
@@ -24615,7 +24623,7 @@
     </row>
     <row r="47" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="60" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B47" s="70"/>
       <c r="C47" s="70"/>
@@ -24647,10 +24655,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" s="71" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C49" s="90" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D49" s="90">
         <f t="shared" ref="D49:G50" si="3">D3*1.05</f>
@@ -24672,7 +24680,7 @@
     <row r="50" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="57"/>
       <c r="B50" s="75" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C50" s="90">
         <f>C4*1.05</f>
@@ -24697,12 +24705,12 @@
     </row>
     <row r="51" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="63" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B52" s="75" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C52" s="90">
         <f t="shared" ref="C52:G55" si="4">C6*1.05</f>
@@ -24727,7 +24735,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B53" s="75" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C53" s="90">
         <f t="shared" si="4"/>
@@ -24752,7 +24760,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="75" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C54" s="90">
         <f t="shared" si="4"/>
@@ -24777,7 +24785,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="75" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C55" s="90">
         <f t="shared" si="4"/>
@@ -24810,7 +24818,7 @@
     </row>
     <row r="57" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="60" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B57" s="70"/>
       <c r="C57" s="70"/>
@@ -24822,7 +24830,7 @@
     <row r="58" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="63"/>
       <c r="B58" s="71" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C58" s="90">
         <f>C12*1.1</f>
@@ -24848,7 +24856,7 @@
     </row>
     <row r="60" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="60" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B60" s="70"/>
       <c r="C60" s="70"/>
@@ -24862,7 +24870,7 @@
         <v>272</v>
       </c>
       <c r="B61" s="75" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C61" s="90">
         <f t="shared" ref="C61:G63" si="5">C15*1.05</f>
@@ -24888,7 +24896,7 @@
     <row r="62" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="57"/>
       <c r="B62" s="75" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C62" s="90">
         <f t="shared" si="5"/>
@@ -24916,7 +24924,7 @@
         <v>111</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C63" s="90">
         <f t="shared" si="5"/>
@@ -24941,7 +24949,7 @@
     </row>
     <row r="65" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="60" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B65" s="70"/>
       <c r="C65" s="70"/>
@@ -24969,7 +24977,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="71" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C67" s="90">
         <f>C21*1.05</f>
@@ -25039,7 +25047,7 @@
         <v>166</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C2" s="90">
         <v>0.21</v>
@@ -25057,7 +25065,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="75"/>
       <c r="B3" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C3" s="90">
         <v>1</v>
@@ -25077,7 +25085,7 @@
         <v>179</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C4" s="90">
         <v>0.15</v>
@@ -25095,7 +25103,7 @@
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="75"/>
       <c r="B5" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C5" s="90">
         <v>1</v>
@@ -25115,7 +25123,7 @@
         <v>180</v>
       </c>
       <c r="B6" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C6" s="90">
         <v>0.15</v>
@@ -25133,7 +25141,7 @@
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="75"/>
       <c r="B7" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C7" s="90">
         <v>1</v>
@@ -25153,7 +25161,7 @@
         <v>181</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C8" s="90">
         <v>0.35</v>
@@ -25171,7 +25179,7 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="75"/>
       <c r="B9" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C9" s="90">
         <v>1</v>
@@ -25191,7 +25199,7 @@
         <v>185</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C10" s="90">
         <v>0.35</v>
@@ -25209,7 +25217,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="75"/>
       <c r="B11" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C11" s="90">
         <v>1</v>
@@ -25229,7 +25237,7 @@
         <v>189</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C12" s="90">
         <v>0.23</v>
@@ -25247,7 +25255,7 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="75"/>
       <c r="B13" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C13" s="90">
         <v>1</v>
@@ -25290,7 +25298,7 @@
         <v>166</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C17" s="90">
         <f t="shared" ref="C17:F28" si="0">C2*0.9</f>
@@ -25312,7 +25320,7 @@
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="75"/>
       <c r="B18" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C18" s="90">
         <f t="shared" si="0"/>
@@ -25336,7 +25344,7 @@
         <v>179</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C19" s="90">
         <f t="shared" si="0"/>
@@ -25358,7 +25366,7 @@
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="75"/>
       <c r="B20" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C20" s="90">
         <f t="shared" si="0"/>
@@ -25382,7 +25390,7 @@
         <v>180</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C21" s="90">
         <f t="shared" si="0"/>
@@ -25404,7 +25412,7 @@
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="75"/>
       <c r="B22" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C22" s="90">
         <f t="shared" si="0"/>
@@ -25428,7 +25436,7 @@
         <v>181</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C23" s="90">
         <f t="shared" si="0"/>
@@ -25450,7 +25458,7 @@
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="75"/>
       <c r="B24" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C24" s="90">
         <f t="shared" si="0"/>
@@ -25474,7 +25482,7 @@
         <v>185</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C25" s="90">
         <f t="shared" si="0"/>
@@ -25496,7 +25504,7 @@
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="75"/>
       <c r="B26" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C26" s="90">
         <f t="shared" si="0"/>
@@ -25520,7 +25528,7 @@
         <v>189</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C27" s="90">
         <f t="shared" si="0"/>
@@ -25542,7 +25550,7 @@
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="75"/>
       <c r="B28" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C28" s="90">
         <f t="shared" si="0"/>
@@ -25589,7 +25597,7 @@
         <v>166</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C32" s="90">
         <f t="shared" ref="C32:F43" si="1">C2*1.05</f>
@@ -25611,7 +25619,7 @@
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="75"/>
       <c r="B33" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C33" s="90">
         <f t="shared" si="1"/>
@@ -25635,7 +25643,7 @@
         <v>179</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C34" s="90">
         <f t="shared" si="1"/>
@@ -25657,7 +25665,7 @@
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="75"/>
       <c r="B35" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C35" s="90">
         <f t="shared" si="1"/>
@@ -25681,7 +25689,7 @@
         <v>180</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C36" s="90">
         <f t="shared" si="1"/>
@@ -25703,7 +25711,7 @@
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="75"/>
       <c r="B37" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C37" s="90">
         <f t="shared" si="1"/>
@@ -25727,7 +25735,7 @@
         <v>181</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C38" s="90">
         <f t="shared" si="1"/>
@@ -25749,7 +25757,7 @@
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="75"/>
       <c r="B39" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C39" s="90">
         <f t="shared" si="1"/>
@@ -25773,7 +25781,7 @@
         <v>185</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C40" s="90">
         <f t="shared" si="1"/>
@@ -25795,7 +25803,7 @@
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="75"/>
       <c r="B41" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C41" s="90">
         <f t="shared" si="1"/>
@@ -25819,7 +25827,7 @@
         <v>189</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C42" s="90">
         <f t="shared" si="1"/>
@@ -25841,7 +25849,7 @@
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="75"/>
       <c r="B43" s="75" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C43" s="90">
         <f t="shared" si="1"/>
@@ -25932,7 +25940,7 @@
     </row>
     <row r="2" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -26509,7 +26517,7 @@
     </row>
     <row r="17" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="57" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B17" s="71"/>
     </row>
@@ -26739,7 +26747,7 @@
     </row>
     <row r="25" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="57" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -27485,7 +27493,7 @@
     </row>
     <row r="40" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="57" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B40" s="71"/>
     </row>
@@ -27767,7 +27775,7 @@
     </row>
     <row r="48" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="57" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -28513,7 +28521,7 @@
     </row>
     <row r="63" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="57" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B63" s="71"/>
     </row>
@@ -28793,7 +28801,7 @@
     </row>
     <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -28818,7 +28826,7 @@
     </row>
     <row r="4" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="120"/>
@@ -28849,7 +28857,7 @@
     </row>
     <row r="7" spans="1:7" s="91" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="91" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -28873,7 +28881,7 @@
     </row>
     <row r="9" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="57" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -28903,7 +28911,7 @@
     </row>
     <row r="11" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="57" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B11" s="71"/>
       <c r="C11" s="120"/>
@@ -28939,7 +28947,7 @@
     </row>
     <row r="14" spans="1:7" s="91" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="91" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -28963,7 +28971,7 @@
     </row>
     <row r="16" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="57" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -28993,7 +29001,7 @@
     </row>
     <row r="18" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="57" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B18" s="71"/>
       <c r="C18" s="120"/>
@@ -29064,10 +29072,10 @@
         <v>156</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C1" s="82" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D1" s="57" t="s">
         <v>67</v>
@@ -29093,7 +29101,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D2" s="90">
         <v>0</v>
@@ -29113,7 +29121,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D3" s="90">
         <v>0</v>
@@ -29133,7 +29141,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D4" s="90">
         <v>0</v>
@@ -29156,10 +29164,10 @@
         <v>191</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D5" s="90">
         <v>0</v>
@@ -29179,7 +29187,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D6" s="90">
         <v>0</v>
@@ -29199,10 +29207,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D7" s="90">
         <v>0</v>
@@ -29222,7 +29230,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D8" s="90">
         <v>0</v>
@@ -29245,10 +29253,10 @@
         <v>184</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D9" s="90">
         <v>0</v>
@@ -29268,7 +29276,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D10" s="90">
         <v>0</v>
@@ -29288,10 +29296,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="90">
         <v>0</v>
@@ -29311,7 +29319,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D12" s="90">
         <v>0</v>
@@ -29334,10 +29342,10 @@
         <v>192</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D13" s="90">
         <v>0</v>
@@ -29357,7 +29365,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D14" s="90">
         <v>0</v>
@@ -29377,10 +29385,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D15" s="90">
         <v>0</v>
@@ -29400,7 +29408,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D16" s="90">
         <v>0</v>
@@ -29423,10 +29431,10 @@
         <v>169</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D17" s="90">
         <v>0</v>
@@ -29446,7 +29454,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D18" s="90">
         <v>0</v>
@@ -29466,10 +29474,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D19" s="90">
         <v>0</v>
@@ -29489,7 +29497,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D20" s="90">
         <v>0</v>
@@ -29515,7 +29523,7 @@
         <v>74</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D21" s="90">
         <v>0.7</v>
@@ -29535,7 +29543,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D22" s="90">
         <v>0.46</v>
@@ -29561,7 +29569,7 @@
         <v>74</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D23" s="90">
         <v>0.7</v>
@@ -29581,7 +29589,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D24" s="90">
         <v>0.46</v>
@@ -29607,7 +29615,7 @@
         <v>74</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D25" s="90">
         <v>0.7</v>
@@ -29627,7 +29635,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D26" s="90">
         <v>0.46</v>
@@ -29653,7 +29661,7 @@
         <v>81</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D27" s="90">
         <v>1</v>
@@ -29673,7 +29681,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D28" s="90">
         <v>0</v>
@@ -29693,7 +29701,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D29" s="90">
         <v>0</v>
@@ -29719,7 +29727,7 @@
         <v>81</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D30" s="90">
         <v>1</v>
@@ -29739,7 +29747,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D31" s="90">
         <v>0</v>
@@ -29759,7 +29767,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D32" s="90">
         <v>0</v>
@@ -29785,7 +29793,7 @@
         <v>81</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D33" s="90">
         <v>1</v>
@@ -29805,7 +29813,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D34" s="90">
         <v>0</v>
@@ -29825,7 +29833,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D35" s="90">
         <v>0</v>
@@ -29851,7 +29859,7 @@
         <v>81</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D36" s="90">
         <v>1</v>
@@ -29871,7 +29879,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D37" s="90">
         <v>0</v>
@@ -29891,7 +29899,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D38" s="90">
         <v>0</v>
@@ -29917,7 +29925,7 @@
         <v>81</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D39" s="90">
         <v>1</v>
@@ -29937,7 +29945,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D40" s="90">
         <v>0</v>
@@ -29957,7 +29965,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D41" s="90">
         <v>0</v>
@@ -29983,7 +29991,7 @@
         <v>81</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D42" s="90">
         <v>0.3</v>
@@ -30003,7 +30011,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D43" s="90">
         <v>0.5</v>
@@ -30023,7 +30031,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D44" s="90">
         <v>0.65</v>
@@ -30046,7 +30054,7 @@
         <v>82</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D45" s="90">
         <v>0.3</v>
@@ -30066,7 +30074,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D46" s="90">
         <v>0.49</v>
@@ -30086,7 +30094,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D47" s="90">
         <v>0.52</v>
@@ -30112,7 +30120,7 @@
         <v>81</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D48" s="90">
         <v>0.88</v>
@@ -30132,7 +30140,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D49" s="90">
         <v>0.93</v>
@@ -30158,7 +30166,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D50" s="90">
         <v>1</v>
@@ -30178,7 +30186,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D51" s="90">
         <v>0.86</v>
@@ -30204,7 +30212,7 @@
         <v>72</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D52" s="90">
         <v>0.57999999999999996</v>
@@ -30224,7 +30232,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D53" s="90">
         <v>0.51</v>
@@ -30244,7 +30252,7 @@
     </row>
     <row r="55" spans="1:8" s="92" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="95" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B55" s="96"/>
       <c r="C55" s="96"/>
@@ -30254,10 +30262,10 @@
         <v>156</v>
       </c>
       <c r="B56" s="57" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C56" s="82" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D56" s="57" t="s">
         <v>67</v>
@@ -30283,7 +30291,7 @@
         <v>81</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D57" s="90">
         <f t="shared" ref="D57:H66" si="0">D2*0.9</f>
@@ -30308,7 +30316,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C58" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D58" s="90">
         <f t="shared" si="0"/>
@@ -30333,7 +30341,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D59" s="90">
         <f t="shared" si="0"/>
@@ -30361,10 +30369,10 @@
         <v>191</v>
       </c>
       <c r="B60" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D60" s="90">
         <f t="shared" si="0"/>
@@ -30389,7 +30397,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C61" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D61" s="90">
         <f t="shared" si="0"/>
@@ -30414,10 +30422,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D62" s="90">
         <f t="shared" si="0"/>
@@ -30442,7 +30450,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C63" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D63" s="90">
         <f t="shared" si="0"/>
@@ -30470,10 +30478,10 @@
         <v>184</v>
       </c>
       <c r="B64" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D64" s="90">
         <f t="shared" si="0"/>
@@ -30498,7 +30506,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C65" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D65" s="90">
         <f t="shared" si="0"/>
@@ -30523,10 +30531,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D66" s="90">
         <f t="shared" si="0"/>
@@ -30551,7 +30559,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C67" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D67" s="90">
         <f t="shared" ref="D67:H76" si="1">D12*0.9</f>
@@ -30579,10 +30587,10 @@
         <v>192</v>
       </c>
       <c r="B68" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D68" s="90">
         <f t="shared" si="1"/>
@@ -30607,7 +30615,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C69" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D69" s="90">
         <f t="shared" si="1"/>
@@ -30632,10 +30640,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D70" s="90">
         <f t="shared" si="1"/>
@@ -30660,7 +30668,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C71" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D71" s="90">
         <f t="shared" si="1"/>
@@ -30688,10 +30696,10 @@
         <v>169</v>
       </c>
       <c r="B72" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D72" s="90">
         <f t="shared" si="1"/>
@@ -30716,7 +30724,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C73" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D73" s="90">
         <f t="shared" si="1"/>
@@ -30741,10 +30749,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C74" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D74" s="90">
         <f t="shared" si="1"/>
@@ -30769,7 +30777,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C75" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D75" s="90">
         <f t="shared" si="1"/>
@@ -30800,7 +30808,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D76" s="90">
         <f t="shared" si="1"/>
@@ -30825,7 +30833,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C77" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D77" s="90">
         <f t="shared" ref="D77:H86" si="2">D22*0.9</f>
@@ -30856,7 +30864,7 @@
         <v>74</v>
       </c>
       <c r="C78" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D78" s="90">
         <f t="shared" si="2"/>
@@ -30881,7 +30889,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C79" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D79" s="90">
         <f t="shared" si="2"/>
@@ -30912,7 +30920,7 @@
         <v>74</v>
       </c>
       <c r="C80" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D80" s="90">
         <f t="shared" si="2"/>
@@ -30937,7 +30945,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C81" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D81" s="90">
         <f t="shared" si="2"/>
@@ -30968,7 +30976,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D82" s="90">
         <f t="shared" si="2"/>
@@ -30993,7 +31001,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C83" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D83" s="90">
         <f t="shared" si="2"/>
@@ -31018,7 +31026,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C84" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D84" s="90">
         <f t="shared" si="2"/>
@@ -31049,7 +31057,7 @@
         <v>81</v>
       </c>
       <c r="C85" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D85" s="90">
         <f t="shared" si="2"/>
@@ -31074,7 +31082,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C86" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D86" s="90">
         <f t="shared" si="2"/>
@@ -31099,7 +31107,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D87" s="90">
         <f t="shared" ref="D87:H96" si="3">D32*0.9</f>
@@ -31130,7 +31138,7 @@
         <v>81</v>
       </c>
       <c r="C88" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D88" s="90">
         <f t="shared" si="3"/>
@@ -31155,7 +31163,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C89" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D89" s="90">
         <f t="shared" si="3"/>
@@ -31180,7 +31188,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C90" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D90" s="90">
         <f t="shared" si="3"/>
@@ -31211,7 +31219,7 @@
         <v>81</v>
       </c>
       <c r="C91" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D91" s="90">
         <f t="shared" si="3"/>
@@ -31236,7 +31244,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D92" s="90">
         <f t="shared" si="3"/>
@@ -31261,7 +31269,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D93" s="90">
         <f t="shared" si="3"/>
@@ -31292,7 +31300,7 @@
         <v>81</v>
       </c>
       <c r="C94" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D94" s="90">
         <f t="shared" si="3"/>
@@ -31317,7 +31325,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C95" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D95" s="90">
         <f t="shared" si="3"/>
@@ -31342,7 +31350,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C96" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D96" s="90">
         <f t="shared" si="3"/>
@@ -31373,7 +31381,7 @@
         <v>81</v>
       </c>
       <c r="C97" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D97" s="90">
         <f t="shared" ref="D97:H106" si="4">D42*0.9</f>
@@ -31398,7 +31406,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C98" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D98" s="90">
         <f t="shared" si="4"/>
@@ -31423,7 +31431,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C99" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D99" s="90">
         <f t="shared" si="4"/>
@@ -31451,7 +31459,7 @@
         <v>82</v>
       </c>
       <c r="C100" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D100" s="90">
         <f t="shared" si="4"/>
@@ -31476,7 +31484,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D101" s="90">
         <f t="shared" si="4"/>
@@ -31501,7 +31509,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D102" s="90">
         <f t="shared" si="4"/>
@@ -31532,7 +31540,7 @@
         <v>81</v>
       </c>
       <c r="C103" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D103" s="90">
         <f t="shared" si="4"/>
@@ -31557,7 +31565,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C104" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D104" s="90">
         <f t="shared" si="4"/>
@@ -31588,7 +31596,7 @@
         <v>81</v>
       </c>
       <c r="C105" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D105" s="90">
         <f t="shared" si="4"/>
@@ -31613,7 +31621,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D106" s="90">
         <f t="shared" si="4"/>
@@ -31644,7 +31652,7 @@
         <v>72</v>
       </c>
       <c r="C107" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D107" s="90">
         <f t="shared" ref="D107:H116" si="5">D52*0.9</f>
@@ -31669,7 +31677,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C108" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D108" s="90">
         <f t="shared" si="5"/>
@@ -31694,7 +31702,7 @@
     </row>
     <row r="110" spans="1:8" s="92" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="95" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B110" s="96"/>
       <c r="C110" s="96"/>
@@ -31704,10 +31712,10 @@
         <v>156</v>
       </c>
       <c r="B111" s="57" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C111" s="82" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D111" s="57" t="s">
         <v>67</v>
@@ -31733,7 +31741,7 @@
         <v>81</v>
       </c>
       <c r="C112" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D112" s="90">
         <f t="shared" ref="D112:H121" si="6">D2*1.05</f>
@@ -31758,7 +31766,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C113" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D113" s="90">
         <f t="shared" si="6"/>
@@ -31783,7 +31791,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C114" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D114" s="90">
         <f t="shared" si="6"/>
@@ -31811,10 +31819,10 @@
         <v>191</v>
       </c>
       <c r="B115" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C115" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D115" s="90">
         <f t="shared" si="6"/>
@@ -31839,7 +31847,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C116" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D116" s="90">
         <f t="shared" si="6"/>
@@ -31864,10 +31872,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B117" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C117" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D117" s="90">
         <f t="shared" si="6"/>
@@ -31892,7 +31900,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C118" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D118" s="90">
         <f t="shared" si="6"/>
@@ -31920,10 +31928,10 @@
         <v>184</v>
       </c>
       <c r="B119" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C119" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D119" s="90">
         <f t="shared" si="6"/>
@@ -31948,7 +31956,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C120" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D120" s="90">
         <f t="shared" si="6"/>
@@ -31973,10 +31981,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B121" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C121" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D121" s="90">
         <f t="shared" si="6"/>
@@ -32001,7 +32009,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C122" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D122" s="90">
         <f t="shared" ref="D122:H131" si="7">D12*1.05</f>
@@ -32029,10 +32037,10 @@
         <v>192</v>
       </c>
       <c r="B123" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C123" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D123" s="90">
         <f t="shared" si="7"/>
@@ -32057,7 +32065,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C124" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D124" s="90">
         <f t="shared" si="7"/>
@@ -32082,10 +32090,10 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C125" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D125" s="90">
         <f t="shared" si="7"/>
@@ -32110,7 +32118,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C126" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D126" s="90">
         <f t="shared" si="7"/>
@@ -32138,10 +32146,10 @@
         <v>169</v>
       </c>
       <c r="B127" s="29" t="s">
-        <v>205</v>
+        <v>342</v>
       </c>
       <c r="C127" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D127" s="90">
         <f t="shared" si="7"/>
@@ -32166,7 +32174,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C128" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D128" s="90">
         <f t="shared" si="7"/>
@@ -32191,10 +32199,10 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="29" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="C129" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D129" s="90">
         <f t="shared" si="7"/>
@@ -32219,7 +32227,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C130" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D130" s="90">
         <f t="shared" si="7"/>
@@ -32250,7 +32258,7 @@
         <v>74</v>
       </c>
       <c r="C131" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D131" s="90">
         <f t="shared" si="7"/>
@@ -32275,7 +32283,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C132" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D132" s="90">
         <f t="shared" ref="D132:H141" si="8">D22*1.05</f>
@@ -32306,7 +32314,7 @@
         <v>74</v>
       </c>
       <c r="C133" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D133" s="90">
         <f t="shared" si="8"/>
@@ -32331,7 +32339,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D134" s="90">
         <f t="shared" si="8"/>
@@ -32362,7 +32370,7 @@
         <v>74</v>
       </c>
       <c r="C135" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D135" s="90">
         <f t="shared" si="8"/>
@@ -32387,7 +32395,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C136" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D136" s="90">
         <f t="shared" si="8"/>
@@ -32418,7 +32426,7 @@
         <v>81</v>
       </c>
       <c r="C137" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D137" s="90">
         <f t="shared" si="8"/>
@@ -32443,7 +32451,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C138" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D138" s="90">
         <f t="shared" si="8"/>
@@ -32468,7 +32476,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C139" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D139" s="90">
         <f t="shared" si="8"/>
@@ -32499,7 +32507,7 @@
         <v>81</v>
       </c>
       <c r="C140" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D140" s="90">
         <f t="shared" si="8"/>
@@ -32524,7 +32532,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C141" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D141" s="90">
         <f t="shared" si="8"/>
@@ -32549,7 +32557,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C142" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D142" s="90">
         <f t="shared" ref="D142:H151" si="9">D32*1.05</f>
@@ -32580,7 +32588,7 @@
         <v>81</v>
       </c>
       <c r="C143" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D143" s="90">
         <f t="shared" si="9"/>
@@ -32605,7 +32613,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C144" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D144" s="90">
         <f t="shared" si="9"/>
@@ -32630,7 +32638,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C145" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D145" s="90">
         <f t="shared" si="9"/>
@@ -32661,7 +32669,7 @@
         <v>81</v>
       </c>
       <c r="C146" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D146" s="90">
         <f t="shared" si="9"/>
@@ -32686,7 +32694,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C147" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D147" s="90">
         <f t="shared" si="9"/>
@@ -32711,7 +32719,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C148" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D148" s="90">
         <f t="shared" si="9"/>
@@ -32742,7 +32750,7 @@
         <v>81</v>
       </c>
       <c r="C149" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D149" s="90">
         <f t="shared" si="9"/>
@@ -32767,7 +32775,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C150" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D150" s="90">
         <f t="shared" si="9"/>
@@ -32792,7 +32800,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C151" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D151" s="90">
         <f t="shared" si="9"/>
@@ -32823,7 +32831,7 @@
         <v>81</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D152" s="90">
         <f t="shared" ref="D152:H161" si="10">D42*1.05</f>
@@ -32848,7 +32856,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C153" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D153" s="90">
         <f t="shared" si="10"/>
@@ -32873,7 +32881,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C154" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D154" s="90">
         <f t="shared" si="10"/>
@@ -32901,7 +32909,7 @@
         <v>82</v>
       </c>
       <c r="C155" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D155" s="90">
         <f t="shared" si="10"/>
@@ -32926,7 +32934,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C156" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D156" s="90">
         <f t="shared" si="10"/>
@@ -32951,7 +32959,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C157" s="29" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D157" s="90">
         <f t="shared" si="10"/>
@@ -32982,7 +32990,7 @@
         <v>81</v>
       </c>
       <c r="C158" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D158" s="90">
         <f t="shared" si="10"/>
@@ -33007,7 +33015,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C159" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D159" s="90">
         <f t="shared" si="10"/>
@@ -33038,7 +33046,7 @@
         <v>81</v>
       </c>
       <c r="C160" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D160" s="90">
         <f t="shared" si="10"/>
@@ -33063,7 +33071,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C161" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D161" s="90">
         <f t="shared" si="10"/>
@@ -33094,7 +33102,7 @@
         <v>72</v>
       </c>
       <c r="C162" s="29" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D162" s="90">
         <f t="shared" ref="D162:H171" si="11">D52*1.05</f>
@@ -33119,7 +33127,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C163" s="29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D163" s="90">
         <f t="shared" si="11"/>
@@ -33175,7 +33183,7 @@
         <v>156</v>
       </c>
       <c r="B1" s="76" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C1" s="76"/>
       <c r="D1" s="57" t="s">
@@ -33200,7 +33208,7 @@
         <v>94</v>
       </c>
       <c r="C2" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D2" s="90">
         <v>1</v>
@@ -33218,7 +33226,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D3" s="90">
         <v>0.2</v>
@@ -33242,7 +33250,7 @@
         <v>94</v>
       </c>
       <c r="C4" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D4" s="90">
         <v>1</v>
@@ -33260,7 +33268,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D5" s="90">
         <v>0.59</v>
@@ -33284,7 +33292,7 @@
         <v>94</v>
       </c>
       <c r="C6" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D6" s="90">
         <v>1</v>
@@ -33302,7 +33310,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D7" s="90">
         <v>0.6</v>
@@ -33320,7 +33328,7 @@
     </row>
     <row r="9" spans="1:8" s="91" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="91" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -33328,7 +33336,7 @@
         <v>156</v>
       </c>
       <c r="B10" s="76" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C10" s="76"/>
       <c r="D10" s="57" t="s">
@@ -33352,7 +33360,7 @@
         <v>94</v>
       </c>
       <c r="C11" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D11" s="90">
         <f t="shared" ref="D11:G16" si="0">D2*0.9</f>
@@ -33373,7 +33381,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D12" s="90">
         <f t="shared" si="0"/>
@@ -33400,7 +33408,7 @@
         <v>94</v>
       </c>
       <c r="C13" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D13" s="90">
         <f t="shared" si="0"/>
@@ -33421,7 +33429,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D14" s="90">
         <f t="shared" si="0"/>
@@ -33448,7 +33456,7 @@
         <v>94</v>
       </c>
       <c r="C15" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D15" s="90">
         <f t="shared" si="0"/>
@@ -33469,7 +33477,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D16" s="90">
         <f t="shared" si="0"/>
@@ -33490,7 +33498,7 @@
     </row>
     <row r="18" spans="1:7" s="91" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.3">
@@ -33498,7 +33506,7 @@
         <v>156</v>
       </c>
       <c r="B19" s="76" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="57" t="s">
@@ -33522,7 +33530,7 @@
         <v>94</v>
       </c>
       <c r="C20" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D20" s="90">
         <f t="shared" ref="D20:G25" si="1">D2*1.05</f>
@@ -33543,7 +33551,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D21" s="90">
         <f t="shared" si="1"/>
@@ -33570,7 +33578,7 @@
         <v>94</v>
       </c>
       <c r="C22" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D22" s="90">
         <f t="shared" si="1"/>
@@ -33591,7 +33599,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D23" s="90">
         <f t="shared" si="1"/>
@@ -33618,7 +33626,7 @@
         <v>94</v>
       </c>
       <c r="C24" s="83" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D24" s="90">
         <f t="shared" si="1"/>
@@ -33639,7 +33647,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="67" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D25" s="90">
         <f t="shared" si="1"/>
@@ -34532,7 +34540,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>